<commit_message>
Spliied data into train and test subsets and evaluated results
</commit_message>
<xml_diff>
--- a/Survey results.xlsx
+++ b/Survey results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Documents\Kasia - Data Analytics course\Projects\DAProg2019\ProgDA_Project2019\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F429BFFA-68EC-49B5-B45C-F60D3DFEDBB4}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3B2EEC5-C834-4338-BC67-8714A60BC7FE}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{1D5031AB-A0DD-4031-9E39-D458977FF3B3}"/>
   </bookViews>
@@ -51,10 +51,10 @@
     <t>Exceeded expectations</t>
   </si>
   <si>
-    <t>Timely query resolution</t>
+    <t>Satisfaction from timely query resolution</t>
   </si>
   <si>
-    <t>Satisfaction from service quality</t>
+    <t>Overall Satisfaction</t>
   </si>
 </sst>
 </file>
@@ -408,8 +408,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{42711E8B-054F-46C6-8E2C-A428938EE182}">
   <dimension ref="A1:D102"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="A27" sqref="A27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -473,7 +473,7 @@
         <v>5</v>
       </c>
       <c r="D4" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.35">
@@ -498,10 +498,10 @@
         <v>5</v>
       </c>
       <c r="C6">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D6" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.35">
@@ -579,13 +579,13 @@
         <v>5</v>
       </c>
       <c r="B12">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C12">
         <v>5</v>
       </c>
       <c r="D12" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.35">
@@ -618,16 +618,16 @@
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A15">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B15">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C15">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D15" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.35">
@@ -646,16 +646,16 @@
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A17">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B17">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C17">
         <v>5</v>
       </c>
       <c r="D17" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.35">
@@ -795,12 +795,12 @@
         <v>5</v>
       </c>
       <c r="D27" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A28">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B28">
         <v>5</v>
@@ -809,21 +809,21 @@
         <v>5</v>
       </c>
       <c r="D28" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A29">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="B29">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="C29">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="D29" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.35">
@@ -898,7 +898,7 @@
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A35">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B35">
         <v>5</v>
@@ -915,10 +915,10 @@
         <v>5</v>
       </c>
       <c r="B36">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C36">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D36" t="s">
         <v>2</v>
@@ -954,27 +954,27 @@
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A39">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="B39">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="C39">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="D39" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A40">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B40">
         <v>5</v>
       </c>
       <c r="C40">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D40" t="s">
         <v>2</v>
@@ -982,13 +982,13 @@
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A41">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="B41">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="C41">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="D41" t="s">
         <v>4</v>
@@ -1010,16 +1010,16 @@
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A43">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B43">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C43">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D43" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.35">
@@ -1033,7 +1033,7 @@
         <v>5</v>
       </c>
       <c r="D44" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.35">
@@ -1047,7 +1047,7 @@
         <v>1</v>
       </c>
       <c r="D45" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.35">
@@ -1061,7 +1061,7 @@
         <v>5</v>
       </c>
       <c r="D46" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.35">
@@ -1072,7 +1072,7 @@
         <v>5</v>
       </c>
       <c r="C47">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D47" t="s">
         <v>2</v>
@@ -1187,7 +1187,7 @@
         <v>1</v>
       </c>
       <c r="D55" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.35">
@@ -1262,13 +1262,13 @@
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A61">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B61">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C61">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D61" t="s">
         <v>2</v>
@@ -1279,13 +1279,13 @@
         <v>5</v>
       </c>
       <c r="B62">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C62">
         <v>4</v>
       </c>
       <c r="D62" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.35">
@@ -1299,7 +1299,7 @@
         <v>1</v>
       </c>
       <c r="D63" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.35">
@@ -1411,7 +1411,7 @@
         <v>5</v>
       </c>
       <c r="D71" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.35">
@@ -1481,7 +1481,7 @@
         <v>5</v>
       </c>
       <c r="D76" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.35">
@@ -1593,7 +1593,7 @@
         <v>5</v>
       </c>
       <c r="D84" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.35">
@@ -1607,7 +1607,7 @@
         <v>5</v>
       </c>
       <c r="D85" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.35">

</xml_diff>